<commit_message>
Sample menu items from Hot Tomato
</commit_message>
<xml_diff>
--- a/CZ2002_MenuItem.xlsx
+++ b/CZ2002_MenuItem.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zhenghao/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zhenghao/Desktop/CZ2002/ASSIGNMENT/CZ2002_RRPSS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Maincourse" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,54 @@
   </si>
   <si>
     <t>Cold</t>
+  </si>
+  <si>
+    <t>Freshly baked bread slices</t>
+  </si>
+  <si>
+    <t>Traditional tasty fries</t>
+  </si>
+  <si>
+    <t>Tasty mashed potato mixed with pepper gravy</t>
+  </si>
+  <si>
+    <t>Nicely fried squid served with special sauce</t>
+  </si>
+  <si>
+    <t>Chicken wings cooked with our special spice</t>
+  </si>
+  <si>
+    <t>Traditional Latte</t>
+  </si>
+  <si>
+    <t>Specially brewed cappuccino</t>
+  </si>
+  <si>
+    <t>Must-try signature espresso coffee</t>
+  </si>
+  <si>
+    <t>Classic Australian coffee</t>
+  </si>
+  <si>
+    <t>Lower suger, more healther</t>
+  </si>
+  <si>
+    <t>Canned soda</t>
+  </si>
+  <si>
+    <t>Freshly juiced with great taste</t>
+  </si>
+  <si>
+    <t>Your perfect coffee mate</t>
+  </si>
+  <si>
+    <t>A fruity iced blend of tropical mango and passion fruit juice with a hibiscus infusion.</t>
+  </si>
+  <si>
+    <t>Classical and unforgettable</t>
+  </si>
+  <si>
+    <t>Scooping happiness to life</t>
   </si>
 </sst>
 </file>
@@ -610,65 +658,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6">
         <v>6.9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -678,18 +744,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,8 +766,11 @@
       <c r="C1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -710,8 +780,11 @@
       <c r="C2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -721,8 +794,11 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -732,8 +808,11 @@
       <c r="C4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -743,8 +822,11 @@
       <c r="C5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -754,8 +836,11 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -765,8 +850,11 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -776,8 +864,11 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -786,6 +877,9 @@
       </c>
       <c r="C9" t="s">
         <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -795,55 +889,71 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5">
         <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>